<commit_message>
add relevancia a plani de teste
</commit_message>
<xml_diff>
--- a/Análise/Nintendo Switch.xlsx
+++ b/Análise/Nintendo Switch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/nicolasmq_al_insper_edu_br/Documents/Insper/2-Semestre/CDados/Projetos/Projeto 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasqueiroga/Desktop/Projeto-1--CDados/Análise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="11_D7B41982A513E03801B03D527959047971663B43" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{35298B1D-7A8A-C841-850B-FD89AE49C978}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8B285E-A678-4A45-8DA9-AA55669289AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="22360" windowHeight="13340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27320" yWindow="-14720" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1504,7 +1503,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1929,12 +1928,12 @@
       <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="255.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1942,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1958,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1990,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2006,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2022,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -2070,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2078,7 +2077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -2110,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2134,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2214,7 +2213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2246,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2270,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2294,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -2382,7 +2381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -2406,7 +2405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -2422,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -2470,7 +2469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>85</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -2678,7 +2677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -2702,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -2718,7 +2717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -2726,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -2742,7 +2741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -2766,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>105</v>
       </c>
@@ -2774,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -2798,7 +2797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -2806,7 +2805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -2814,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>114</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -2854,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>117</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -2886,7 +2885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -2902,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>125</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>126</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>127</v>
       </c>
@@ -2951,7 +2950,7 @@
       </c>
       <c r="F127" s="5"/>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>128</v>
       </c>
@@ -2959,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>129</v>
       </c>
@@ -2967,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>130</v>
       </c>
@@ -2975,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>131</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>132</v>
       </c>
@@ -2991,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>133</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>134</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>135</v>
       </c>
@@ -3015,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>136</v>
       </c>
@@ -3023,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>137</v>
       </c>
@@ -3031,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>138</v>
       </c>
@@ -3039,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>139</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>140</v>
       </c>
@@ -3055,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>141</v>
       </c>
@@ -3063,7 +3062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>142</v>
       </c>
@@ -3071,7 +3070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>143</v>
       </c>
@@ -3079,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>145</v>
       </c>
@@ -3095,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>146</v>
       </c>
@@ -3103,7 +3102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>147</v>
       </c>
@@ -3111,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>148</v>
       </c>
@@ -3119,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -3127,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>150</v>
       </c>
@@ -3135,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>151</v>
       </c>
@@ -3143,7 +3142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>152</v>
       </c>
@@ -3151,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>153</v>
       </c>
@@ -3159,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>154</v>
       </c>
@@ -3167,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>155</v>
       </c>
@@ -3175,7 +3174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>156</v>
       </c>
@@ -3183,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>157</v>
       </c>
@@ -3191,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>158</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>159</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>160</v>
       </c>
@@ -3215,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>161</v>
       </c>
@@ -3223,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>162</v>
       </c>
@@ -3231,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>163</v>
       </c>
@@ -3239,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>164</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>165</v>
       </c>
@@ -3255,7 +3254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>166</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>167</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>168</v>
       </c>
@@ -3279,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>169</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>170</v>
       </c>
@@ -3295,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>171</v>
       </c>
@@ -3303,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>172</v>
       </c>
@@ -3311,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>173</v>
       </c>
@@ -3319,7 +3318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>174</v>
       </c>
@@ -3327,7 +3326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>175</v>
       </c>
@@ -3335,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>176</v>
       </c>
@@ -3343,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>177</v>
       </c>
@@ -3351,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>178</v>
       </c>
@@ -3359,7 +3358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>179</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>180</v>
       </c>
@@ -3375,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>181</v>
       </c>
@@ -3383,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>182</v>
       </c>
@@ -3391,7 +3390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -3399,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>184</v>
       </c>
@@ -3407,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>185</v>
       </c>
@@ -3415,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>186</v>
       </c>
@@ -3423,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>187</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>188</v>
       </c>
@@ -3439,7 +3438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>189</v>
       </c>
@@ -3447,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>190</v>
       </c>
@@ -3455,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>191</v>
       </c>
@@ -3463,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>192</v>
       </c>
@@ -3471,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>193</v>
       </c>
@@ -3479,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>194</v>
       </c>
@@ -3487,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>195</v>
       </c>
@@ -3495,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>196</v>
       </c>
@@ -3503,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>197</v>
       </c>
@@ -3511,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>198</v>
       </c>
@@ -3519,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>199</v>
       </c>
@@ -3527,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>200</v>
       </c>
@@ -3535,7 +3534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>201</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>202</v>
       </c>
@@ -3551,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>203</v>
       </c>
@@ -3559,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>204</v>
       </c>
@@ -3567,7 +3566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>205</v>
       </c>
@@ -3575,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>206</v>
       </c>
@@ -3583,7 +3582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>207</v>
       </c>
@@ -3591,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>208</v>
       </c>
@@ -3599,7 +3598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>209</v>
       </c>
@@ -3607,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>210</v>
       </c>
@@ -3615,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>211</v>
       </c>
@@ -3623,7 +3622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>212</v>
       </c>
@@ -3631,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>213</v>
       </c>
@@ -3639,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>214</v>
       </c>
@@ -3647,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>215</v>
       </c>
@@ -3655,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>216</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>217</v>
       </c>
@@ -3671,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>218</v>
       </c>
@@ -3679,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>219</v>
       </c>
@@ -3687,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>220</v>
       </c>
@@ -3695,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>221</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>222</v>
       </c>
@@ -3711,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>223</v>
       </c>
@@ -3719,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>224</v>
       </c>
@@ -3727,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>225</v>
       </c>
@@ -3735,7 +3734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>226</v>
       </c>
@@ -3743,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>227</v>
       </c>
@@ -3751,7 +3750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>228</v>
       </c>
@@ -3759,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>229</v>
       </c>
@@ -3767,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>230</v>
       </c>
@@ -3775,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>231</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>232</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>233</v>
       </c>
@@ -3799,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>234</v>
       </c>
@@ -3807,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>235</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>236</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>237</v>
       </c>
@@ -3831,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>238</v>
       </c>
@@ -3839,7 +3838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>239</v>
       </c>
@@ -3847,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>240</v>
       </c>
@@ -3855,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>241</v>
       </c>
@@ -3863,7 +3862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>242</v>
       </c>
@@ -3871,7 +3870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>243</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>244</v>
       </c>
@@ -3887,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>245</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>246</v>
       </c>
@@ -3903,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>247</v>
       </c>
@@ -3911,7 +3910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>248</v>
       </c>
@@ -3919,7 +3918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>249</v>
       </c>
@@ -3927,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>250</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>251</v>
       </c>
@@ -3943,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>252</v>
       </c>
@@ -3951,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>253</v>
       </c>
@@ -3959,7 +3958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>254</v>
       </c>
@@ -3967,7 +3966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>255</v>
       </c>
@@ -3975,7 +3974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>256</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>257</v>
       </c>
@@ -3991,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>258</v>
       </c>
@@ -3999,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>259</v>
       </c>
@@ -4007,7 +4006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>260</v>
       </c>
@@ -4015,7 +4014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>261</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>262</v>
       </c>
@@ -4031,7 +4030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>263</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>264</v>
       </c>
@@ -4047,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>265</v>
       </c>
@@ -4055,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>266</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>267</v>
       </c>
@@ -4071,7 +4070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>268</v>
       </c>
@@ -4079,7 +4078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>269</v>
       </c>
@@ -4087,7 +4086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>270</v>
       </c>
@@ -4095,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>271</v>
       </c>
@@ -4103,7 +4102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>272</v>
       </c>
@@ -4111,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>273</v>
       </c>
@@ -4119,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>274</v>
       </c>
@@ -4127,7 +4126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>275</v>
       </c>
@@ -4135,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>276</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>277</v>
       </c>
@@ -4151,7 +4150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>278</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>279</v>
       </c>
@@ -4167,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>280</v>
       </c>
@@ -4175,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>281</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>282</v>
       </c>
@@ -4191,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>283</v>
       </c>
@@ -4199,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>284</v>
       </c>
@@ -4207,7 +4206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>285</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>286</v>
       </c>
@@ -4223,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>287</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>288</v>
       </c>
@@ -4239,7 +4238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>289</v>
       </c>
@@ -4247,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>290</v>
       </c>
@@ -4255,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>291</v>
       </c>
@@ -4263,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>292</v>
       </c>
@@ -4271,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>293</v>
       </c>
@@ -4279,7 +4278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>294</v>
       </c>
@@ -4287,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>295</v>
       </c>
@@ -4295,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>296</v>
       </c>
@@ -4303,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>297</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>298</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>299</v>
       </c>
@@ -4327,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>300</v>
       </c>
@@ -4335,7 +4334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>301</v>
       </c>
@@ -4355,17 +4354,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="122" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="247" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>302</v>
       </c>
@@ -4373,599 +4372,956 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>421</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>